<commit_message>
replace nfdi4pso for dpbo terms in DNA extraction template
</commit_message>
<xml_diff>
--- a/templates/dataplant/2EXT04_DNA.xlsx
+++ b/templates/dataplant/2EXT04_DNA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\SWATE_templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\sciebo - Eggels, Stella (s.eggels@fz-juelich.de)@fz-juelich.sciebo.de\SE\DataPLANT\ARCs und SWATE\ersatz von nfdi4pso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D733EE7-40FD-4EEC-B9BB-0138D89897D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AAFC9B-8CD3-43F7-B3D4-95894CFC53B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="19110" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-96" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT04_DNA" sheetId="1" r:id="rId1"/>
@@ -51,75 +51,75 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B81F90EA-1EA7-4FF0-9CEC-2E77DFDBC937}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The unique identifier of this template. It will be auto generated.
-Reply:
+Antwort:
     id=a927fd4c-851f-4a69-8aa0-fc680f495a64</t>
       </text>
     </comment>
     <comment ref="A2" authorId="1" shapeId="0" xr:uid="{19FA76EE-58A6-4624-8AC3-08B90C032C24}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate template.</t>
       </text>
     </comment>
     <comment ref="A3" authorId="2" shapeId="0" xr:uid="{A85942F5-9D9D-45C2-A4C7-2451DB92B494}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The current version of this template in SemVer notation.</t>
       </text>
     </comment>
     <comment ref="A4" authorId="3" shapeId="0" xr:uid="{98079BCD-9E2A-4078-BB94-3F580328B80F}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The description of this template. Use few sentences for succinctness.</t>
       </text>
     </comment>
     <comment ref="A5" authorId="4" shapeId="0" xr:uid="{794CE9E5-1451-44C7-9160-78ACFB17B1C1}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
       </text>
     </comment>
     <comment ref="A6" authorId="5" shapeId="0" xr:uid="{5ABC23F5-5754-4F65-9E1E-CA015DE37348}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate annotation table in the workbook of the template's excel file.</t>
       </text>
     </comment>
     <comment ref="A7" authorId="6" shapeId="0" xr:uid="{11BF48F2-3D63-4F79-A9B9-FA5AD485DB78}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A11" authorId="7" shapeId="0" xr:uid="{77E425D2-2A27-475E-8D60-F54201D62D82}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all tags associated with this template. Tags are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A15" authorId="8" shapeId="0" xr:uid="{AE101BCE-4FC9-4469-B553-EF8695E9D747}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The author(s) of this template.</t>
       </text>
     </comment>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="91">
   <si>
     <t>Source Name</t>
   </si>
@@ -136,57 +136,9 @@
     <t>Sample Name</t>
   </si>
   <si>
-    <t>Parameter [Bio entity]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000012)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000012)</t>
-  </si>
-  <si>
-    <t>Parameter [Biosource amount]</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:0000013)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000013)</t>
-  </si>
-  <si>
-    <t>Parameter [Extraction method]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000054)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000054)</t>
-  </si>
-  <si>
-    <t>Parameter [Extraction buffer]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000050)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000050)</t>
-  </si>
-  <si>
-    <t>Parameter [Extraction buffer volume]</t>
-  </si>
-  <si>
-    <t>Unit (#2)</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000051)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000051)</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -328,39 +280,6 @@
     <t>Review comments</t>
   </si>
   <si>
-    <t>NFDI4PSO:0000012</t>
-  </si>
-  <si>
-    <t>NFDI4PSO</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000012</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000013</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000013</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000054</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000054</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000050</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000050</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000051</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000051</t>
-  </si>
-  <si>
     <t>RNA (Transcriptomics)</t>
   </si>
   <si>
@@ -382,33 +301,9 @@
     <t>phenol:chloroform:isopropanol</t>
   </si>
   <si>
-    <t>user-specific</t>
-  </si>
-  <si>
     <t>protein</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000093</t>
-  </si>
-  <si>
-    <t>milligram</t>
-  </si>
-  <si>
-    <t>UO</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000022</t>
-  </si>
-  <si>
-    <t>microliter</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000101</t>
-  </si>
-  <si>
-    <t>1.1.6</t>
-  </si>
-  <si>
     <t>Authors ORCID</t>
   </si>
   <si>
@@ -422,6 +317,90 @@
   </si>
   <si>
     <t>DataPLANT</t>
+  </si>
+  <si>
+    <t>Parameter [bio entity]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000012)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000012)</t>
+  </si>
+  <si>
+    <t>Parameter [biosource amount]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000013)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000013)</t>
+  </si>
+  <si>
+    <t>Parameter [extraction method]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000054)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000054)</t>
+  </si>
+  <si>
+    <t>Parameter [extraction buffer]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000050)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000050)</t>
+  </si>
+  <si>
+    <t>Parameter [extraction buffer volume]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit </t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000051)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000051)</t>
+  </si>
+  <si>
+    <t>1.1.7</t>
+  </si>
+  <si>
+    <t>DPBO:0000012</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000012</t>
+  </si>
+  <si>
+    <t>DPBO:0000013</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000013</t>
+  </si>
+  <si>
+    <t>DPBO</t>
+  </si>
+  <si>
+    <t>DPBO:0000054</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000054</t>
+  </si>
+  <si>
+    <t>DPBO:0000050</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000050</t>
+  </si>
+  <si>
+    <t>DPBO:0000051</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000051</t>
   </si>
 </sst>
 </file>
@@ -456,10 +435,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -588,11 +569,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -632,53 +614,64 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{DE2A6450-71E8-47E2-B297-E4C3E22BB7A5}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -705,23 +698,23 @@
   <autoFilter ref="A1:S5" xr:uid="{86110337-507F-400B-9E37-176F907029D7}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{2D4FFDA4-6A76-42E5-BD93-D89F35B78BBA}" name="Source Name"/>
-    <tableColumn id="3" xr3:uid="{CE1F3C26-D51E-45C1-A5BC-DFB94FFD541A}" name="Parameter [Bio entity]"/>
-    <tableColumn id="4" xr3:uid="{928603B1-DF6F-4B58-80EF-55E176034F49}" name="Term Source REF (NFDI4PSO:0000012)"/>
-    <tableColumn id="5" xr3:uid="{E78AA681-40BD-4A6C-8B4E-BCF9AD53C719}" name="Term Accession Number (NFDI4PSO:0000012)"/>
-    <tableColumn id="6" xr3:uid="{CF5C6027-24FC-45F9-9767-152CA533F0B0}" name="Parameter [Biosource amount]" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{EEB4CD46-928A-4C7C-A9BC-E1C6257CECF4}" name="Unit" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{59858248-740C-4BB1-8CCC-9A2C087FFFBB}" name="Term Source REF (NFDI4PSO:0000013)" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{84A9113B-5B76-4DBF-AD81-7426BDFA7ECF}" name="Term Accession Number (NFDI4PSO:0000013)" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{503EADCF-3D61-402C-B794-CDC1CE0F3DB8}" name="Parameter [Extraction method]" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{B3B8F0EF-CF9C-4F10-BFCB-F8A24073D054}" name="Term Source REF (NFDI4PSO:0000054)" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{A26E2839-B090-4297-B720-A6D467DE2F13}" name="Term Accession Number (NFDI4PSO:0000054)" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{A9345EE2-EAE1-4A40-B39B-EDD0F168C40B}" name="Parameter [Extraction buffer]" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{E8F1F34D-A150-4A24-8E2F-D67DEA72AFA7}" name="Term Source REF (NFDI4PSO:0000050)" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{22B9817D-BD35-4A87-8C7C-4047B579332A}" name="Term Accession Number (NFDI4PSO:0000050)" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{1433C27D-F7EC-437F-B05D-4FD4A4E39319}" name="Parameter [Extraction buffer volume]" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{8814589D-7786-4616-BEB5-4ADBB2890EF7}" name="Unit (#2)" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{9DB32C00-681C-45EB-AA4C-12127D4B9AA0}" name="Term Source REF (NFDI4PSO:0000051)" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{378FB1CC-F188-4DF3-9C18-2D67D932AE32}" name="Term Accession Number (NFDI4PSO:0000051)" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{3D1DC7BA-AB6B-48BE-97FF-EFD89F76EA84}" name="Parameter [bio entity]"/>
+    <tableColumn id="4" xr3:uid="{12F7FB7B-9755-40E0-A711-699393D542EA}" name="Term Source REF (DPBO:0000012)" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{DE5FDCD7-627B-4165-B187-04FFC255D31C}" name="Term Accession Number (DPBO:0000012)" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{4A98E45D-46B3-415C-8EB1-A54FBBA1A674}" name="Parameter [biosource amount]" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{65B8B250-4B54-4FC2-B43B-C3BAF69B40DA}" name="Unit" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{754F8090-7B1D-4AD5-9ADD-938594F662A5}" name="Term Source REF (DPBO:0000013)" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{DBFC685F-738E-42D7-BB58-27BDAE1F4029}" name="Term Accession Number (DPBO:0000013)" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{15B9AD90-CFF6-436F-978D-0E1931CAAA93}" name="Parameter [extraction method]" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{21270944-F9FC-4931-B327-46C000F433C9}" name="Term Source REF (DPBO:0000054)" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{C0A2B38D-DA5E-4800-A08D-50F2D2377CA1}" name="Term Accession Number (DPBO:0000054)" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{A8489B05-AF9F-462A-83BD-53C822988AE1}" name="Parameter [extraction buffer]" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{F4855B13-FE93-4CBF-A3B3-B7CEDA49F3B0}" name="Term Source REF (DPBO:0000050)" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{9B287147-A869-4F61-989F-729EFC83B57E}" name="Term Accession Number (DPBO:0000050)" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{C875B7F2-5868-4743-9C4F-BEDB5CCD070D}" name="Parameter [extraction buffer volume]" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{77C15429-C137-45FB-A49C-BE83046FFFAC}" name="Unit " dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{9046D909-BD86-46AD-9DA0-E1DE8667359D}" name="Term Source REF (DPBO:0000051)" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{F110696F-A619-48B0-8A17-86CB4EE5DA17}" name="Term Accession Number (DPBO:0000051)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{5A83D931-1161-4B00-BE33-39C7AF2CE0AB}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1026,7 +1019,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="655" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="676" row="2">
@@ -1059,262 +1052,286 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.21875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="J1" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="K1" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="L1" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="M1" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="O1" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="P1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="Q1" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="R1" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="S1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>84</v>
+        <v>50</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>84</v>
+        <v>55</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="O2" s="2">
         <v>200</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>84</v>
+        <v>51</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>91</v>
+        <v>57</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1329,223 +1346,223 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B230FA2-6BAA-4C1F-9634-19942CC6AE92}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="C16" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -1560,329 +1577,338 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>5</v>
-      </c>
       <c r="B5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="B6" s="14" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>12</v>
-      </c>
       <c r="B7" s="14" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>74</v>
+        <v>84</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>76</v>
+        <v>84</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{C3F37371-BFFD-48B0-BE55-A9D0142ABE55}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{76925293-32AA-47FC-A11C-9B3287EA12F2}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{1DB17764-E999-421F-8C52-6CB7CCA0CCC7}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{8E3C642B-3665-459C-ACD7-EE90EBE04C34}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{E62D0CD5-85D9-48F4-921D-BEF8AB1171AB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>